<commit_message>
creating my first Keyword driven framework
</commit_message>
<xml_diff>
--- a/Tutorial/Utilities & Configuration/DataEngine.xlsx
+++ b/Tutorial/Utilities & Configuration/DataEngine.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="20550" windowHeight="4725"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Steps" sheetId="1" r:id="rId1"/>
-    <sheet name="Test Cases" sheetId="2" r:id="rId2"/>
+    <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
+    <sheet name="Test Steps" sheetId="1" r:id="rId2"/>
     <sheet name="Settings" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -518,9 +518,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -708,63 +765,6 @@
       </c>
       <c r="G9" t="s">
         <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>